<commit_message>
atualizando dados de marcação e recaptura do piloto
</commit_message>
<xml_diff>
--- a/Ago2022.xlsx
+++ b/Ago2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\Mestrado\Projeto\Mestrado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27857B12-778C-45E5-ABA7-1CF6A1710FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783D716F-B260-409E-85E9-65E1F003CF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -687,7 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F58056C-D756-4BCE-93BB-D7A4F835FA99}">
   <dimension ref="A1:D356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
       <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>

</xml_diff>